<commit_message>
com caminhos falta o resto
</commit_message>
<xml_diff>
--- a/ExcelToXML_DB_Converter/Excel/2024/Bring_Pensoes_RV_2024.12.xlsx
+++ b/ExcelToXML_DB_Converter/Excel/2024/Bring_Pensoes_RV_2024.12.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Desktop\TaniaAlmeida-FichRH\AON\hhh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Documents\BringGlobal\ExcelToXML_DB_Converter\Excel\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1800094-A56A-4F74-8261-22E96C6D3AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE55588-1881-4AB7-8105-A1302061B08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,9 +109,6 @@
     <t>NIPC Empresa</t>
   </si>
   <si>
-    <t>Empresa</t>
-  </si>
-  <si>
     <t>Nome</t>
   </si>
   <si>
@@ -191,6 +188,9 @@
   </si>
   <si>
     <t>x2@bringglobal.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empresa </t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1017,7 @@
       <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,52 +1163,52 @@
         <v>19</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="P4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="Q4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="R4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="S4" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="S4" s="14" t="s">
-        <v>35</v>
       </c>
       <c r="T4" s="15"/>
       <c r="U4" s="6"/>
@@ -1223,7 +1223,7 @@
       <c r="Z4" s="46"/>
       <c r="AA4" s="6"/>
       <c r="AB4" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:28" s="21" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -1231,37 +1231,37 @@
         <v>100000088</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="36" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="23"/>
       <c r="H5" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M5" s="24"/>
       <c r="N5" s="23">
         <v>43833</v>
       </c>
       <c r="O5" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P5" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q5" s="26"/>
       <c r="R5" s="11"/>
@@ -1289,37 +1289,37 @@
         <v>100000089</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="23"/>
       <c r="H6" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" s="24"/>
       <c r="N6" s="23">
         <v>43497</v>
       </c>
       <c r="O6" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P6" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q6" s="26"/>
       <c r="R6" s="11"/>

</xml_diff>